<commit_message>
Assignemnet 4 Arrays Find Duplicate and RU Rotten tomatoes git add .git add .BE CAREFUL WHEN READING SPECIFICATIONS AND WRT ROW MAJOR vs COL MAJOR ORDER
</commit_message>
<xml_diff>
--- a/FALL-2022/INTRO_TO_CS/Grades.xlsx
+++ b/FALL-2022/INTRO_TO_CS/Grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/792b544d67660648/Documents/CLASS/FALL-2022/INTRO_TO_CS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="11_F25DC773A252ABDACC10482021997DB45ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1F0F6F8-AC8B-4D01-B731-7C9719CF2A83}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_F25DC773A252ABDACC10482021997DB45ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3068F35E-768B-4ADB-87A7-E110097BCB16}"/>
   <bookViews>
-    <workbookView xWindow="11310" yWindow="6195" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homework" sheetId="1" r:id="rId1"/>
@@ -117,6 +117,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -180,6 +183,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -654,10 +660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F328EE69-D2F7-4AF5-8826-BF04CC8A0572}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,6 +707,9 @@
       <c r="C2" s="1">
         <v>150</v>
       </c>
+      <c r="D2" s="1">
+        <v>145</v>
+      </c>
       <c r="E2" s="5">
         <v>1</v>
       </c>
@@ -746,6 +755,16 @@
       <c r="C5" s="2">
         <f>SUM(C2:C4)</f>
         <v>450</v>
+      </c>
+      <c r="D5" s="1">
+        <f>SUM(D2:D4)</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="7">
+        <f>D5/SUMIF(D2:D4,"&gt;0",C2:C4)</f>
+        <v>0.96666666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -757,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CAC383-68F7-4A7A-B00E-A62745B94138}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Week 9 Recursion Sierpinski
</commit_message>
<xml_diff>
--- a/FALL-2022/INTRO_TO_CS/Grades.xlsx
+++ b/FALL-2022/INTRO_TO_CS/Grades.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/792b544d67660648/Documents/CLASS/FALL-2022/INTRO_TO_CS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="11_F25DC773A252ABDACC10482021997DB45ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F9CA970-B801-404A-AFBE-802896F9263F}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="11_F25DC773A252ABDACC10482021997DB45ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5DEA5F2-C075-4250-9408-1CDE4FF8D764}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homework" sheetId="1" r:id="rId1"/>
     <sheet name="Exams" sheetId="2" r:id="rId2"/>
-    <sheet name="Weeks" sheetId="4" r:id="rId3"/>
-    <sheet name="Recitation" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Weeks" sheetId="4" r:id="rId4"/>
+    <sheet name="Recitation" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>Assignment</t>
   </si>
@@ -120,6 +121,57 @@
   </si>
   <si>
     <t>Exam grade</t>
+  </si>
+  <si>
+    <t>Pre-Recitation Quiz</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Out Of</t>
+  </si>
+  <si>
+    <t>Post-Recitation Quiz</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>Wind Chill</t>
+  </si>
+  <si>
+    <t>Order Check</t>
+  </si>
+  <si>
+    <t>Largest of Five</t>
+  </si>
+  <si>
+    <t>Check Digit</t>
+  </si>
+  <si>
+    <t>Random Walker</t>
+  </si>
+  <si>
+    <t>Exam</t>
+  </si>
+  <si>
+    <t>Find Duplicate</t>
+  </si>
+  <si>
+    <t>RU Rotten Tomatoes</t>
+  </si>
+  <si>
+    <t>Polygon Transform</t>
+  </si>
+  <si>
+    <t>Sierpinski</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Extra Credit</t>
   </si>
 </sst>
 </file>
@@ -174,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -197,6 +249,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F328EE69-D2F7-4AF5-8826-BF04CC8A0572}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -827,6 +880,547 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE788A47-8DF8-4328-991E-848EEEA4956E}">
+  <dimension ref="A1:E42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <f>B4+1</f>
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <f>B5+1</f>
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <f>B6+1</f>
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <f>B7+1</f>
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <f>B8+1</f>
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ref="B10:B15" si="0">B9+1</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <f>B16+1</f>
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <f>B17+1</f>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <f>B18+1</f>
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <f>B19+1</f>
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <f>B20+1</f>
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <f>B21+1</f>
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <f>B22+1</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <f>B23+1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <f>B24+1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <f>B25+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <f>B26+1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <f>B27+1</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>34.71</v>
+      </c>
+      <c r="D29">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+      <c r="D33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>30</v>
+      </c>
+      <c r="D34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>30</v>
+      </c>
+      <c r="D37">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>25</v>
+      </c>
+      <c r="D38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>127.5</v>
+      </c>
+      <c r="D41">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f>SUM(C2:C41)</f>
+        <v>367.21000000000004</v>
+      </c>
+      <c r="D42">
+        <f>SUM(D2:D41)</f>
+        <v>402</v>
+      </c>
+      <c r="E42" s="8">
+        <f>C42/D42</f>
+        <v>0.9134577114427862</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CAC383-68F7-4A7A-B00E-A62745B94138}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -984,7 +1578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C97070F-79A6-47DA-B6F9-1931419129DB}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Recursion Example 2.3.4 Htrees pg 277
</commit_message>
<xml_diff>
--- a/FALL-2022/INTRO_TO_CS/Grades.xlsx
+++ b/FALL-2022/INTRO_TO_CS/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/792b544d67660648/Documents/CLASS/FALL-2022/INTRO_TO_CS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="11_F25DC773A252ABDACC10482021997DB45ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C6A6ABA-EEA6-4432-B6C6-4449180FB6FD}"/>
+  <xr:revisionPtr revIDLastSave="507" documentId="11_F25DC773A252ABDACC10482021997DB45ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CB4D6AE-0C0A-4552-9120-635580D081E1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,9 @@
     <sheet name="Homework" sheetId="1" r:id="rId1"/>
     <sheet name="Exams" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="Weeks" sheetId="4" r:id="rId4"/>
-    <sheet name="Recitation" sheetId="3" r:id="rId5"/>
+    <sheet name="EXAM 2" sheetId="6" r:id="rId4"/>
+    <sheet name="Weeks" sheetId="4" r:id="rId5"/>
+    <sheet name="Recitation" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="73">
   <si>
     <t>Assignment</t>
   </si>
@@ -199,6 +200,66 @@
   </si>
   <si>
     <t>margin left</t>
+  </si>
+  <si>
+    <t>Days Remaining</t>
+  </si>
+  <si>
+    <t>Chapters</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>Static Methods</t>
+  </si>
+  <si>
+    <t>Libraries and Clients</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Day/Ch</t>
+  </si>
+  <si>
+    <t>Review Material</t>
+  </si>
+  <si>
+    <t>Ch</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Lecture Slides</t>
+  </si>
+  <si>
+    <t>Lecture Questions</t>
+  </si>
+  <si>
+    <t>Reciation Questions</t>
+  </si>
+  <si>
+    <t>Practice Exam</t>
+  </si>
+  <si>
+    <t>F22</t>
+  </si>
+  <si>
+    <t>S23</t>
+  </si>
+  <si>
+    <t>Self-Test</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -254,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -271,12 +332,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -317,13 +396,25 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -960,7 +1051,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,17 +1141,17 @@
         <f t="shared" ref="E3:E41" si="0">C3-D3</f>
         <v>0</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="9">
         <v>850</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="9">
         <f t="shared" ref="I3:I6" si="1">H3-1000</f>
         <v>-150</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="10">
         <f t="shared" ref="J3:J6" si="2">I3-$E$43</f>
         <v>-133.71</v>
       </c>
@@ -1750,6 +1841,12 @@
       <c r="B39" s="1">
         <v>10</v>
       </c>
+      <c r="C39" s="1">
+        <v>50</v>
+      </c>
+      <c r="D39" s="1">
+        <v>50</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1775,10 +1872,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="1">
-        <v>127.5</v>
+        <v>130.5</v>
       </c>
       <c r="D41" s="1">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="0"/>
@@ -1788,11 +1885,11 @@
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <f>SUM(C2:C41)</f>
-        <v>397.71000000000004</v>
+        <v>450.71000000000004</v>
       </c>
       <c r="D42" s="1">
         <f>SUM(D2:D41)</f>
-        <v>419</v>
+        <v>472</v>
       </c>
       <c r="E42" s="1">
         <f>SUM(E2:E41)</f>
@@ -1800,7 +1897,7 @@
       </c>
       <c r="F42" s="7">
         <f>C42/D42</f>
-        <v>0.94918854415274467</v>
+        <v>0.95489406779661024</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1816,6 +1913,600 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D126FB8C-47FA-4B56-B9F6-F1E0C91D8287}">
+  <dimension ref="A1:I38"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <f ca="1">TODAY()</f>
+        <v>44865</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="18">
+        <v>1.4</v>
+      </c>
+      <c r="I2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <f ca="1">A2+1</f>
+        <v>44866</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="1">
+        <f>H2+0.1</f>
+        <v>1.5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <f t="shared" ref="A4:A18" ca="1" si="0">A3+1</f>
+        <v>44867</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44868</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H7" si="1">H4+0.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44869</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="20">
+        <f t="shared" si="1"/>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44870</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="15">
+        <f>COUNT(D2:D6)</f>
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44871</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="1">
+        <f ca="1">ROUNDDOWN(B19/E7,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="1">
+        <f>H7+0.1</f>
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44872</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44873</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" ref="H10:H11" si="2">H9+0.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44874</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="20">
+        <f t="shared" si="2"/>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44875</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44876</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="1">
+        <f>H12+0.1</f>
+        <v>1.5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44877</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44878</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" ref="H15:H16" si="3">H14+0.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44879</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="20">
+        <f t="shared" si="3"/>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44880</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>44881</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="1">
+        <f>H17+0.1</f>
+        <v>1.5</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="15">
+        <f ca="1">COUNT(A2:A18)</f>
+        <v>17</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" ref="H20:H21" si="4">H19+0.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G21" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="20">
+        <f t="shared" si="4"/>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="I22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="1">
+        <f>H22+0.1</f>
+        <v>1.5</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:H26" si="5">H24+0.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" s="20">
+        <f t="shared" si="5"/>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="I26" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="G30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" s="1">
+        <f>H29+0.1</f>
+        <v>1.5</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" ref="H32:H33" si="6">H31+0.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G33" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H33" s="20">
+        <f t="shared" si="6"/>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="I34" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" s="1">
+        <f>H34+0.1</f>
+        <v>1.5</v>
+      </c>
+      <c r="I35" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="I36" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" ref="H37:H38" si="7">H36+0.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I37" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="7"/>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="I38" s="1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CAC383-68F7-4A7A-B00E-A62745B94138}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -1973,7 +2664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C97070F-79A6-47DA-B6F9-1931419129DB}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
added folders for spirng semester
</commit_message>
<xml_diff>
--- a/FALL-2022/INTRO_TO_CS/Grades.xlsx
+++ b/FALL-2022/INTRO_TO_CS/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/792b544d67660648/Documents/CLASS/FALL-2022/INTRO_TO_CS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="575" documentId="11_F25DC773A252ABDACC10482021997DB45ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69CD782D-46CD-4EB8-82BA-C30417270148}"/>
+  <xr:revisionPtr revIDLastSave="578" documentId="11_F25DC773A252ABDACC10482021997DB45ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3E22388-A5B2-4F23-98BE-A90BF695D968}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,7 +275,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -373,7 +373,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -432,16 +432,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1091,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE788A47-8DF8-4328-991E-848EEEA4956E}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1165,7 @@
       </c>
       <c r="K2" s="13">
         <f>J2-$E$48</f>
-        <v>-67.710000000000008</v>
+        <v>-63.71</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1204,7 +1201,7 @@
       </c>
       <c r="K3" s="10">
         <f>J3-$E$48</f>
-        <v>-117.71000000000001</v>
+        <v>-113.71000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1241,7 +1238,7 @@
       </c>
       <c r="K4" s="10">
         <f>J4-$E$48</f>
-        <v>-167.71</v>
+        <v>-163.71</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1278,7 +1275,7 @@
       </c>
       <c r="K5" s="10">
         <f>J5-$E$48</f>
-        <v>-217.71</v>
+        <v>-213.71</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1315,7 +1312,7 @@
       </c>
       <c r="K6" s="10">
         <f>J6-$E$48</f>
-        <v>-267.70999999999998</v>
+        <v>-263.70999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1558,11 +1555,17 @@
       <c r="C17" s="1">
         <v>0</v>
       </c>
+      <c r="D17" s="1">
+        <v>4</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="6"/>
+        <v>-4</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1726,24 +1729,24 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="24">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="C25" s="25">
-        <v>4</v>
-      </c>
-      <c r="D25" s="25">
-        <v>4</v>
-      </c>
-      <c r="E25" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="26">
+      <c r="C25" s="24">
+        <v>4</v>
+      </c>
+      <c r="D25" s="24">
+        <v>4</v>
+      </c>
+      <c r="E25" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="25">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2104,23 +2107,23 @@
       <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="23">
-        <v>1</v>
-      </c>
-      <c r="C44" s="23">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1">
         <v>130.5</v>
       </c>
-      <c r="D44" s="23">
+      <c r="D44" s="1">
         <v>150</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E44" s="1">
         <f t="shared" si="0"/>
         <v>-19.5</v>
       </c>
-      <c r="F44" s="24">
+      <c r="F44" s="23">
         <f t="shared" si="1"/>
         <v>0.87</v>
       </c>
@@ -2156,18 +2159,18 @@
       </c>
       <c r="C46" s="20">
         <f>D46*F46</f>
-        <v>82.289999999999992</v>
+        <v>86.289999999999992</v>
       </c>
       <c r="D46" s="8">
         <v>150</v>
       </c>
       <c r="E46" s="8">
         <f t="shared" si="6"/>
-        <v>-67.710000000000008</v>
+        <v>-63.710000000000008</v>
       </c>
       <c r="F46" s="22">
         <f>(D45+K2)/D45</f>
-        <v>0.54859999999999998</v>
+        <v>0.57526666666666659</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2177,26 +2180,26 @@
       </c>
       <c r="D47" s="1">
         <f>SUM(D2:D44)</f>
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="E47" s="1">
         <f>SUM(E2:E45)</f>
-        <v>-37.29</v>
+        <v>-41.29</v>
       </c>
       <c r="F47" s="6">
         <f t="shared" si="1"/>
-        <v>0.95385093167701873</v>
+        <v>0.94601642710472289</v>
       </c>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D48" s="6">
         <f>C47/D47</f>
-        <v>0.95385093167701873</v>
+        <v>0.94601642710472289</v>
       </c>
       <c r="E48" s="1">
         <f>E47+5</f>
-        <v>-32.29</v>
+        <v>-36.29</v>
       </c>
     </row>
   </sheetData>
@@ -2248,7 +2251,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <f ca="1">TODAY()</f>
-        <v>44882</v>
+        <v>44888</v>
       </c>
       <c r="D2" s="1">
         <v>1.4</v>
@@ -2269,7 +2272,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f ca="1">A2+1</f>
-        <v>44883</v>
+        <v>44889</v>
       </c>
       <c r="D3" s="1">
         <v>1.5</v>
@@ -2291,7 +2294,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A18" ca="1" si="0">A3+1</f>
-        <v>44884</v>
+        <v>44890</v>
       </c>
       <c r="D4" s="1">
         <v>2.1</v>
@@ -2312,7 +2315,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44885</v>
+        <v>44891</v>
       </c>
       <c r="D5" s="1">
         <v>2.2000000000000002</v>
@@ -2334,7 +2337,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44886</v>
+        <v>44892</v>
       </c>
       <c r="D6" s="1">
         <v>2.2999999999999998</v>
@@ -2356,7 +2359,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44887</v>
+        <v>44893</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>59</v>
@@ -2378,7 +2381,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44888</v>
+        <v>44894</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>60</v>
@@ -2401,7 +2404,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44889</v>
+        <v>44895</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>64</v>
@@ -2416,7 +2419,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44890</v>
+        <v>44896</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>64</v>
@@ -2432,7 +2435,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44891</v>
+        <v>44897</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>64</v>
@@ -2448,7 +2451,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44892</v>
+        <v>44898</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>65</v>
@@ -2463,7 +2466,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44893</v>
+        <v>44899</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>65</v>
@@ -2479,7 +2482,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44894</v>
+        <v>44900</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>65</v>
@@ -2494,7 +2497,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44895</v>
+        <v>44901</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>65</v>
@@ -2510,7 +2513,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44896</v>
+        <v>44902</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>65</v>
@@ -2526,7 +2529,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44897</v>
+        <v>44903</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>66</v>
@@ -2541,7 +2544,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>44898</v>
+        <v>44904</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>66</v>

</xml_diff>